<commit_message>
* ## BUGFIXES E NOVOS ITENS ##
* Corrigido bug que tornava a consulta por leituras já efetuadas muito
* lentas devido a joins mal indexados
* Adicionado botão para Cancelar leitura atual para ser possível iniciar
* uma nova.
* Corrigidos bugs de funcionalidades dependentes entre os Controles que
* não possuiam todas as chamadas de código individualmente, como o
* controle de Fechamento de Lote
* Incluido Novos Bins na documentacao e no Script de atualizacao da base
* de dados
</commit_message>
<xml_diff>
--- a/doctos/BINS_Losango.xlsx
+++ b/doctos/BINS_Losango.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="141">
   <si>
     <t>ORG</t>
   </si>
@@ -811,15 +811,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="3"/>
     <col min="3" max="3" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
@@ -2591,12 +2591,397 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>407</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>407</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>407</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>407</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>407</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>407</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>407</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>407</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>407</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>407</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>407</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>407</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>407</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>407</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>407</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>407</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>407</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>407</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>407</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>407</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>407</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>407</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>407</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>407</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>407</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>407</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>

</xml_diff>